<commit_message>
Update Rumaway Tasklist - GameJam.xlsx
</commit_message>
<xml_diff>
--- a/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
+++ b/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C2240950\Documents\GitHub\Pun-Panik_GameJam\Shared Documentation\Luke's Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21392163-D914-4826-AF25-ED4F80352223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1303E5-BA58-4575-8B7C-134285377EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13050" yWindow="3180" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Rumaway Tasks:</t>
   </si>
@@ -97,6 +97,51 @@
   </si>
   <si>
     <t>Level:</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>playable</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Populating</t>
+  </si>
+  <si>
+    <t>Booze Pickup</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>luke</t>
+  </si>
+  <si>
+    <t>works. just needs better visual + self delete</t>
+  </si>
+  <si>
+    <t>got speed boost, needs other bonus</t>
+  </si>
+  <si>
+    <t>Research:</t>
+  </si>
+  <si>
+    <t>(Bar) Level Research</t>
+  </si>
+  <si>
+    <t>Prop Research</t>
   </si>
 </sst>
 </file>
@@ -457,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,122 +513,192 @@
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="22.140625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="15.85546875" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="D14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1st Population+ task edit
</commit_message>
<xml_diff>
--- a/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
+++ b/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C2240950\Documents\GitHub\Pun-Panik_GameJam\Shared Documentation\Luke's Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E494C3-DD7A-4881-ACCC-77D4B59B8FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E1598-24E9-482B-AB34-22D2C80F4628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Rumaway Tasks:</t>
   </si>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +581,9 @@
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
ai & pick up gamefeel
</commit_message>
<xml_diff>
--- a/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
+++ b/Shared Documentation/Luke's Docs/Rumaway Tasklist - GameJam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C2240950\Documents\GitHub\Pun-Panik_GameJam\Shared Documentation\Luke's Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB15811-5A95-4C2C-B263-3D94D4ADB44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6097A-0F11-41FD-B4CC-8BE515EB1A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Rumaway Tasks:</t>
   </si>
@@ -156,9 +156,6 @@
     <t>optional</t>
   </si>
   <si>
-    <t>Asthetic:</t>
-  </si>
-  <si>
     <t>passable</t>
   </si>
   <si>
@@ -186,13 +183,28 @@
     <t>1st attempt</t>
   </si>
   <si>
-    <t>get mouse to work when dead</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
     <t>top</t>
+  </si>
+  <si>
+    <t>get mouse to work</t>
+  </si>
+  <si>
+    <t>Aesthetic:</t>
+  </si>
+  <si>
+    <t>Gameplay objects</t>
+  </si>
+  <si>
+    <t>could be more efficient</t>
+  </si>
+  <si>
+    <t>worked too well - finetune</t>
+  </si>
+  <si>
+    <t>AI Behavior</t>
   </si>
 </sst>
 </file>
@@ -567,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +602,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>9</v>
@@ -617,7 +629,7 @@
         <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,7 +668,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -667,28 +679,28 @@
         <v>24</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -705,7 +717,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -715,7 +727,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -723,7 +735,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -762,13 +774,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>27</v>
@@ -786,7 +798,7 @@
         <v>32</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -808,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,23 +831,29 @@
         <v>42</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>55</v>
+      <c r="D26" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -845,7 +863,7 @@
         <v>15</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,9 +881,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,12 +900,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>